<commit_message>
The problem was that (for some reason) index/INDEX is a reserved word and can't be used in "ORDER BY" (even though "name" is also a reserved word and that *can* be used in "ORDER BY"). Solution: use "id" instead of "index".
</commit_message>
<xml_diff>
--- a/data/SortByTest.xlsx
+++ b/data/SortByTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="0" windowWidth="25600" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="TheTable" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <t>three</t>
   </si>
   <si>
-    <t>index</t>
+    <t>id</t>
   </si>
 </sst>
 </file>
@@ -446,7 +446,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>